<commit_message>
Fixed bugs in displaying car info, now displaying NHTSA info (need to format)
</commit_message>
<xml_diff>
--- a/Cars2/CarFieldsTemplate.xlsx
+++ b/Cars2/CarFieldsTemplate.xlsx
@@ -15,8 +15,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eric Ruff</author>
+  </authors>
+  <commentList>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eric Ruff:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Show 'make_display' if it exists, otherwise 'make'.
+This is hardcoded.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="104">
   <si>
     <t xml:space="preserve">                    {{ car.id }} -</t>
   </si>
@@ -283,14 +319,80 @@
   </si>
   <si>
     <t>car-grp</t>
+  </si>
+  <si>
+    <t>{{ car.make_display ? car.make_display : car.make }}</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>NHTSACampaignNumber</t>
+  </si>
+  <si>
+    <t>ReportReceivedDate</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Conequence</t>
+  </si>
+  <si>
+    <t>Remedy</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>ModelYear</t>
+  </si>
+  <si>
+    <t>NHTSA Campaign Number</t>
+  </si>
+  <si>
+    <t>Report Received Date</t>
+  </si>
+  <si>
+    <t>Consequence</t>
+  </si>
+  <si>
+    <t>Model Year</t>
+  </si>
+  <si>
+    <t>recall-grp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -318,9 +420,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -623,85 +729,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="61" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="E2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -737,8 +847,8 @@
         <v>&lt;/span&gt;</v>
       </c>
       <c r="I4" t="str">
-        <f>"&lt;"&amp;$F$1&amp;" class=""car-data"" &gt;"</f>
-        <v>&lt;span class="car-data" &gt;</v>
+        <f>"&lt;"&amp;$F$1&amp;" class=""car-data {{carView.cars[0].d_" &amp; F4 &amp; "}}"" &gt;"</f>
+        <v>&lt;span class="car-data {{carView.cars[0].d_id}}" &gt;</v>
       </c>
       <c r="J4" t="str">
         <f>"{{ car."&amp;D4&amp;" ? "&amp;"car."&amp;D4&amp;" : ""n/a"" }}"</f>
@@ -750,7 +860,7 @@
       </c>
       <c r="L4" t="str">
         <f>"&lt;div class=""" &amp; $L$1&amp;""" &gt;"&amp;E4&amp;G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;"&lt;/div&gt;"</f>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Id&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.id ? car.id : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Id&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_id}}" &gt;{{ car.id ? car.id : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -785,20 +895,19 @@
         <v>&lt;/span&gt;</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5:I40" si="6">"&lt;"&amp;$F$1&amp;" class=""car-data"" &gt;"</f>
-        <v>&lt;span class="car-data" &gt;</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" ref="J5:J40" si="7">"{{ car."&amp;D5&amp;" ? "&amp;"car."&amp;D5&amp;" : ""n/a"" }}"</f>
-        <v>{{ car.make ? car.make : "n/a" }}</v>
+        <f t="shared" ref="I5:I40" si="6">"&lt;"&amp;$F$1&amp;" class=""car-data {{carView.cars[0].d_" &amp; F5 &amp; "}}"" &gt;"</f>
+        <v>&lt;span class="car-data {{carView.cars[0].d_make}}" &gt;</v>
+      </c>
+      <c r="J5" t="s">
+        <v>89</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K40" si="8">"&lt;/"&amp;$F$1&amp;"&gt;"</f>
+        <f t="shared" ref="K5:K40" si="7">"&lt;/"&amp;$F$1&amp;"&gt;"</f>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" ref="L5:L40" si="9">"&lt;div class=""" &amp; $L$1&amp;""" &gt;"&amp;E5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;"&lt;/div&gt;"</f>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Make&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.make ? car.make : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="L5:L40" si="8">"&lt;div class=""" &amp; $L$1&amp;""" &gt;"&amp;E5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Make&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_make}}" &gt;{{ car.make_display ? car.make_display : car.make }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -834,19 +943,19 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_model_name}}" &gt;</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="J6:J40" si="9">"{{ car."&amp;D6&amp;" ? "&amp;"car."&amp;D6&amp;" : ""n/a"" }}"</f>
         <v>{{ car.model_name ? car.model_name : "n/a" }}</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Model&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.model_name ? car.model_name : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Model&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_model_name}}" &gt;{{ car.model_name ? car.model_name : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -882,19 +991,19 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_model_trim}}" &gt;</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.model_trim ? car.model_trim : "n/a" }}</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Trim&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.model_trim ? car.model_trim : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Trim&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_model_trim}}" &gt;{{ car.model_trim ? car.model_trim : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -930,19 +1039,19 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_model_year}}" &gt;</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.model_year ? car.model_year : "n/a" }}</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Year&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.model_year ? car.model_year : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Year&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_model_year}}" &gt;{{ car.model_year ? car.model_year : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -978,19 +1087,19 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_body_style}}" &gt;</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.body_style ? car.body_style : "n/a" }}</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Body style&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.body_style ? car.body_style : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Body style&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_body_style}}" &gt;{{ car.body_style ? car.body_style : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1026,19 +1135,19 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_position}}" &gt;</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_position ? car.engine_position : "n/a" }}</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Engine position&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_position ? car.engine_position : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Engine position&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_position}}" &gt;{{ car.engine_position ? car.engine_position : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1074,19 +1183,19 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_cc}}" &gt;</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_cc ? car.engine_cc : "n/a" }}</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Engine cc&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_cc ? car.engine_cc : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Engine cc&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_cc}}" &gt;{{ car.engine_cc ? car.engine_cc : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1122,19 +1231,19 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_num_cyl}}" &gt;</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_num_cyl ? car.engine_num_cyl : "n/a" }}</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Num cylinders&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_num_cyl ? car.engine_num_cyl : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Num cylinders&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_num_cyl}}" &gt;{{ car.engine_num_cyl ? car.engine_num_cyl : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1170,19 +1279,19 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_type}}" &gt;</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_type ? car.engine_type : "n/a" }}</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Engine type&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_type ? car.engine_type : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Engine type&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_type}}" &gt;{{ car.engine_type ? car.engine_type : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1218,19 +1327,19 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_valves_per_cyl}}" &gt;</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_valves_per_cyl ? car.engine_valves_per_cyl : "n/a" }}</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Valves per cyl&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_valves_per_cyl ? car.engine_valves_per_cyl : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Valves per cyl&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_valves_per_cyl}}" &gt;{{ car.engine_valves_per_cyl ? car.engine_valves_per_cyl : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1266,19 +1375,19 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_power_ps}}" &gt;</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_power_ps ? car.engine_power_ps : "n/a" }}</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Horsepower&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_power_ps ? car.engine_power_ps : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Horsepower&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_power_ps}}" &gt;{{ car.engine_power_ps ? car.engine_power_ps : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1314,19 +1423,19 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_power_rpm}}" &gt;</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_power_rpm ? car.engine_power_rpm : "n/a" }}</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Power - rpm&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_power_rpm ? car.engine_power_rpm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Power - rpm&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_power_rpm}}" &gt;{{ car.engine_power_rpm ? car.engine_power_rpm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1362,19 +1471,19 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_torque_nm}}" &gt;</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_torque_nm ? car.engine_torque_nm : "n/a" }}</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Power - torque&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_torque_nm ? car.engine_torque_nm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Power - torque&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_torque_nm}}" &gt;{{ car.engine_torque_nm ? car.engine_torque_nm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1410,19 +1519,19 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_torque_rpm}}" &gt;</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_torque_rpm ? car.engine_torque_rpm : "n/a" }}</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Torque rpm&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_torque_rpm ? car.engine_torque_rpm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Torque rpm&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_torque_rpm}}" &gt;{{ car.engine_torque_rpm ? car.engine_torque_rpm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,19 +1567,19 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_bore_mm}}" &gt;</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_bore_mm ? car.engine_bore_mm : "n/a" }}</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Bore (mm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_bore_mm ? car.engine_bore_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Bore (mm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_bore_mm}}" &gt;{{ car.engine_bore_mm ? car.engine_bore_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1506,19 +1615,19 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_stroke_mm}}" &gt;</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_stroke_mm ? car.engine_stroke_mm : "n/a" }}</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Stroke (mm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_stroke_mm ? car.engine_stroke_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Stroke (mm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_stroke_mm}}" &gt;{{ car.engine_stroke_mm ? car.engine_stroke_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1554,19 +1663,19 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_compression}}" &gt;</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_compression ? car.engine_compression : "n/a" }}</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Compression ratio&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_compression ? car.engine_compression : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Compression ratio&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_compression}}" &gt;{{ car.engine_compression ? car.engine_compression : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1602,19 +1711,19 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_engine_fuel}}" &gt;</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.engine_fuel ? car.engine_fuel : "n/a" }}</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Fuel&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.engine_fuel ? car.engine_fuel : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Fuel&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_engine_fuel}}" &gt;{{ car.engine_fuel ? car.engine_fuel : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1650,19 +1759,19 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_top_speed_kph}}" &gt;</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.top_speed_kph ? car.top_speed_kph : "n/a" }}</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Top speed (kph)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.top_speed_kph ? car.top_speed_kph : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Top speed (kph)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_top_speed_kph}}" &gt;{{ car.top_speed_kph ? car.top_speed_kph : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1698,19 +1807,19 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_zero_to_100_kph}}" &gt;</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.zero_to_100_kph ? car.zero_to_100_kph : "n/a" }}</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Zero to 100kph&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.zero_to_100_kph ? car.zero_to_100_kph : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Zero to 100kph&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_zero_to_100_kph}}" &gt;{{ car.zero_to_100_kph ? car.zero_to_100_kph : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1746,19 +1855,19 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_drive_type}}" &gt;</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.drive_type ? car.drive_type : "n/a" }}</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Drive type&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.drive_type ? car.drive_type : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Drive type&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_drive_type}}" &gt;{{ car.drive_type ? car.drive_type : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1794,19 +1903,19 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_transmission_type}}" &gt;</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.transmission_type ? car.transmission_type : "n/a" }}</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Transmission type&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.transmission_type ? car.transmission_type : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Transmission type&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_transmission_type}}" &gt;{{ car.transmission_type ? car.transmission_type : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1842,19 +1951,19 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_seats}}" &gt;</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.seats ? car.seats : "n/a" }}</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;# seats&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.seats ? car.seats : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;# seats&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_seats}}" &gt;{{ car.seats ? car.seats : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1890,19 +1999,19 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_doors}}" &gt;</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.doors ? car.doors : "n/a" }}</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;# doors&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.doors ? car.doors : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;# doors&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_doors}}" &gt;{{ car.doors ? car.doors : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1938,19 +2047,19 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_weight_kg}}" &gt;</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.weight_kg ? car.weight_kg : "n/a" }}</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Weight (kg)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.weight_kg ? car.weight_kg : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Weight (kg)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_weight_kg}}" &gt;{{ car.weight_kg ? car.weight_kg : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1986,19 +2095,19 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_length_mm}}" &gt;</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.length_mm ? car.length_mm : "n/a" }}</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Length (mm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.length_mm ? car.length_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Length (mm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_length_mm}}" &gt;{{ car.length_mm ? car.length_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2034,19 +2143,19 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_width_mm}}" &gt;</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.width_mm ? car.width_mm : "n/a" }}</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Width (mm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.width_mm ? car.width_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Width (mm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_width_mm}}" &gt;{{ car.width_mm ? car.width_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2082,19 +2191,19 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_height_mm}}" &gt;</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.height_mm ? car.height_mm : "n/a" }}</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Height (mm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.height_mm ? car.height_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Height (mm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_height_mm}}" &gt;{{ car.height_mm ? car.height_mm : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2130,19 +2239,19 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_wheelbase}}" &gt;</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.wheelbase ? car.wheelbase : "n/a" }}</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Wheelbase&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.wheelbase ? car.wheelbase : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Wheelbase&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_wheelbase}}" &gt;{{ car.wheelbase ? car.wheelbase : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2178,19 +2287,19 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_lkm_hwy}}" &gt;</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.lkm_hwy ? car.lkm_hwy : "n/a" }}</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Highway (lkm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.lkm_hwy ? car.lkm_hwy : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Highway (lkm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_lkm_hwy}}" &gt;{{ car.lkm_hwy ? car.lkm_hwy : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2226,19 +2335,19 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_lkm_mixed}}" &gt;</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.lkm_mixed ? car.lkm_mixed : "n/a" }}</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Mixed (lkm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.lkm_mixed ? car.lkm_mixed : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Mixed (lkm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_lkm_mixed}}" &gt;{{ car.lkm_mixed ? car.lkm_mixed : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2274,19 +2383,19 @@
       </c>
       <c r="I36" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_lkm_city}}" &gt;</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.lkm_city ? car.lkm_city : "n/a" }}</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;City (lkm)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.lkm_city ? car.lkm_city : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;City (lkm)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_lkm_city}}" &gt;{{ car.lkm_city ? car.lkm_city : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2322,19 +2431,19 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_fuel_capacity_l}}" &gt;</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.fuel_capacity_l ? car.fuel_capacity_l : "n/a" }}</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Fuel capacity (l)&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.fuel_capacity_l ? car.fuel_capacity_l : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Fuel capacity (l)&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_fuel_capacity_l}}" &gt;{{ car.fuel_capacity_l ? car.fuel_capacity_l : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2370,19 +2479,19 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_sold_in_us}}" &gt;</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.sold_in_us ? car.sold_in_us : "n/a" }}</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Sold in U.S.&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.sold_in_us ? car.sold_in_us : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Sold in U.S.&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_sold_in_us}}" &gt;{{ car.sold_in_us ? car.sold_in_us : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2418,19 +2527,19 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_co2}}" &gt;</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.co2 ? car.co2 : "n/a" }}</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;CO2&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.co2 ? car.co2 : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;CO2&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_co2}}" &gt;{{ car.co2 ? car.co2 : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2466,23 +2575,385 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;span class="car-data" &gt;</v>
+        <v>&lt;span class="car-data {{carView.cars[0].d_make_display}}" &gt;</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{{ car.make_display ? car.make_display : "n/a" }}</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>&lt;/span&gt;</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Make&lt;/span&gt;&lt;span class="car-data" &gt;{{ car.make_display ? car.make_display : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f t="shared" si="8"/>
+        <v>&lt;div class="car-grp" &gt;&lt;span class="car-heading" &gt;Make&lt;/span&gt;&lt;span class="car-data {{carView.cars[0].d_make_display}}" &gt;{{ car.make_display ? car.make_display : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E46" t="str">
+        <f>"&lt;"&amp;$F$1&amp;" class=""recall-heading"" &gt;"</f>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F46" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" ref="H46:H56" si="10">"&lt;/"&amp;$F$1&amp;"&gt;"</f>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I46" t="str">
+        <f>"&lt;"&amp;$F$1&amp;" class=""recall-data"" &gt;"</f>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J46" t="str">
+        <f>"{{ notice."&amp;F46&amp;" ? "&amp;"notice."&amp;F46&amp;" : ""n/a"" }}"</f>
+        <v>{{ notice.Manufacturer ? notice.Manufacturer : "n/a" }}</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" ref="K46:K56" si="11">"&lt;/"&amp;$F$1&amp;"&gt;"</f>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L46" t="str">
+        <f>"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E46&amp;G46&amp;H46&amp;I46&amp;J46&amp;K46&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Make&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Manufacturer ? notice.Manufacturer : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" t="str">
+        <f t="shared" ref="E47:E56" si="12">"&lt;"&amp;$F$1&amp;" class=""recall-heading"" &gt;"</f>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F47" t="s">
+        <v>91</v>
+      </c>
+      <c r="G47" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" ref="I47:I56" si="13">"&lt;"&amp;$F$1&amp;" class=""recall-data"" &gt;"</f>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" ref="J47:J56" si="14">"{{ notice."&amp;F47&amp;" ? "&amp;"notice."&amp;F47&amp;" : ""n/a"" }}"</f>
+        <v>{{ notice.NHTSACampaignNumber ? notice.NHTSACampaignNumber : "n/a" }}</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" ref="L47:L56" si="15">"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E47&amp;G47&amp;H47&amp;I47&amp;J47&amp;K47&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;NHTSA Campaign Number&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.NHTSACampaignNumber ? notice.NHTSACampaignNumber : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E48" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" t="s">
+        <v>100</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.ReportReceivedDate ? notice.ReportReceivedDate : "n/a" }}</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Report Received Date&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.ReportReceivedDate ? notice.ReportReceivedDate : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E49" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F49" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" t="s">
+        <v>93</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Component ? notice.Component : "n/a" }}</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Component&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Component ? notice.Component : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E50" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F50" t="s">
+        <v>94</v>
+      </c>
+      <c r="G50" t="s">
+        <v>94</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Summary ? notice.Summary : "n/a" }}</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Summary&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Summary ? notice.Summary : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E51" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
+      </c>
+      <c r="G51" t="s">
+        <v>101</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Conequence ? notice.Conequence : "n/a" }}</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Consequence&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Conequence ? notice.Conequence : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E52" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F52" t="s">
+        <v>96</v>
+      </c>
+      <c r="G52" t="s">
+        <v>96</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Remedy ? notice.Remedy : "n/a" }}</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Remedy&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Remedy ? notice.Remedy : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E53" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F53" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" t="s">
+        <v>97</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Notes ? notice.Notes : "n/a" }}</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Notes&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Notes ? notice.Notes : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E54" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F54" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.ModelYear ? notice.ModelYear : "n/a" }}</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Model Year&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.ModelYear ? notice.ModelYear : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E55" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F55" t="s">
+        <v>52</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Make ? notice.Make : "n/a" }}</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Make&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Make ? notice.Make : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E56" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;span class="recall-heading" &gt;</v>
+      </c>
+      <c r="F56" t="s">
+        <v>53</v>
+      </c>
+      <c r="G56" t="s">
+        <v>53</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;span class="recall-data" &gt;</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="14"/>
+        <v>{{ notice.Model ? notice.Model : "n/a" }}</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/span&gt;</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Model&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Model ? notice.Model : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Almost finished! All images display, looks clean
</commit_message>
<xml_diff>
--- a/Cars2/CarFieldsTemplate.xlsx
+++ b/Cars2/CarFieldsTemplate.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
   <si>
     <t xml:space="preserve">                    {{ car.id }} -</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>recall-grp</t>
+  </si>
+  <si>
+    <t>Recall notice elements:</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -732,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" topLeftCell="I21" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,356 +2604,364 @@
         <v>103</v>
       </c>
     </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E46" t="str">
-        <f>"&lt;"&amp;$F$1&amp;" class=""recall-heading"" &gt;"</f>
-        <v>&lt;span class="recall-heading" &gt;</v>
+        <f>"&lt;"&amp;$H$45&amp;" class=""recall-heading"" &gt;"</f>
+        <v>&lt;p class="recall-heading" &gt;</v>
       </c>
       <c r="F46" t="s">
         <v>90</v>
       </c>
       <c r="G46" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" ref="H46:H56" si="10">"&lt;/"&amp;$F$1&amp;"&gt;"</f>
-        <v>&lt;/span&gt;</v>
+        <f>"&lt;/"&amp;$H$45&amp;"&gt;"</f>
+        <v>&lt;/p&gt;</v>
       </c>
       <c r="I46" t="str">
-        <f>"&lt;"&amp;$F$1&amp;" class=""recall-data"" &gt;"</f>
-        <v>&lt;span class="recall-data" &gt;</v>
+        <f>"&lt;"&amp;$H$45&amp;" class=""recall-data"" &gt;"</f>
+        <v>&lt;p class="recall-data" &gt;</v>
       </c>
       <c r="J46" t="str">
         <f>"{{ notice."&amp;F46&amp;" ? "&amp;"notice."&amp;F46&amp;" : ""n/a"" }}"</f>
         <v>{{ notice.Manufacturer ? notice.Manufacturer : "n/a" }}</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" ref="K46:K56" si="11">"&lt;/"&amp;$F$1&amp;"&gt;"</f>
-        <v>&lt;/span&gt;</v>
+        <f>"&lt;/"&amp;$H$45&amp;"&gt;"</f>
+        <v>&lt;/p&gt;</v>
       </c>
       <c r="L46" t="str">
         <f>"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E46&amp;G46&amp;H46&amp;I46&amp;J46&amp;K46&amp;"&lt;/div&gt;"</f>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Make&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Manufacturer ? notice.Manufacturer : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Manufacturer&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Manufacturer ? notice.Manufacturer : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E47" t="str">
-        <f t="shared" ref="E47:E56" si="12">"&lt;"&amp;$F$1&amp;" class=""recall-heading"" &gt;"</f>
-        <v>&lt;span class="recall-heading" &gt;</v>
+        <f t="shared" ref="E47:E56" si="10">"&lt;"&amp;$H$45&amp;" class=""recall-heading"" &gt;"</f>
+        <v>&lt;p class="recall-heading" &gt;</v>
       </c>
       <c r="F47" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G47" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
+        <f t="shared" ref="H47:H56" si="11">"&lt;/"&amp;$H$45&amp;"&gt;"</f>
+        <v>&lt;/p&gt;</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" ref="I47:I56" si="13">"&lt;"&amp;$F$1&amp;" class=""recall-data"" &gt;"</f>
-        <v>&lt;span class="recall-data" &gt;</v>
+        <f t="shared" ref="I47:I56" si="12">"&lt;"&amp;$H$45&amp;" class=""recall-data"" &gt;"</f>
+        <v>&lt;p class="recall-data" &gt;</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" ref="J47:J56" si="14">"{{ notice."&amp;F47&amp;" ? "&amp;"notice."&amp;F47&amp;" : ""n/a"" }}"</f>
-        <v>{{ notice.NHTSACampaignNumber ? notice.NHTSACampaignNumber : "n/a" }}</v>
+        <f>"{{ notice."&amp;F47&amp;" ? "&amp;"notice."&amp;F47&amp;" : ""n/a"" }}"</f>
+        <v>{{ notice.ModelYear ? notice.ModelYear : "n/a" }}</v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
+        <f t="shared" ref="K47:K56" si="13">"&lt;/"&amp;$H$45&amp;"&gt;"</f>
+        <v>&lt;/p&gt;</v>
       </c>
       <c r="L47" t="str">
-        <f t="shared" ref="L47:L56" si="15">"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E47&amp;G47&amp;H47&amp;I47&amp;J47&amp;K47&amp;"&lt;/div&gt;"</f>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;NHTSA Campaign Number&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.NHTSACampaignNumber ? notice.NHTSACampaignNumber : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <f>"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E47&amp;G47&amp;H47&amp;I47&amp;J47&amp;K47&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Model Year&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.ModelYear ? notice.ModelYear : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E48" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F48" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I48" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F48" t="s">
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J48" t="str">
+        <f>"{{ notice."&amp;F48&amp;" ? "&amp;"notice."&amp;F48&amp;" : ""n/a"" }}"</f>
+        <v>{{ notice.Make ? notice.Make : "n/a" }}</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L48" t="str">
+        <f>"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E48&amp;G48&amp;H48&amp;I48&amp;J48&amp;K48&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Make&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Make ? notice.Make : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E49" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F49" t="s">
+        <v>53</v>
+      </c>
+      <c r="G49" t="s">
+        <v>53</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J49" t="str">
+        <f>"{{ notice."&amp;F49&amp;" ? "&amp;"notice."&amp;F49&amp;" : ""n/a"" }}"</f>
+        <v>{{ notice.Model ? notice.Model : "n/a" }}</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L49" t="str">
+        <f>"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E49&amp;G49&amp;H49&amp;I49&amp;J49&amp;K49&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Model&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Model ? notice.Model : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E50" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F50" t="s">
+        <v>91</v>
+      </c>
+      <c r="G50" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" ref="J50:J56" si="14">"{{ notice."&amp;F50&amp;" ? "&amp;"notice."&amp;F50&amp;" : ""n/a"" }}"</f>
+        <v>{{ notice.NHTSACampaignNumber ? notice.NHTSACampaignNumber : "n/a" }}</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" ref="L50:L56" si="15">"&lt;div class=""" &amp; $L$44&amp;""" &gt;"&amp;E50&amp;G50&amp;H50&amp;I50&amp;J50&amp;K50&amp;"&lt;/div&gt;"</f>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;NHTSA Campaign Number&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.NHTSACampaignNumber ? notice.NHTSACampaignNumber : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E51" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F51" t="s">
         <v>92</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G51" t="s">
         <v>100</v>
       </c>
-      <c r="H48" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I48" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J48" t="str">
+      <c r="H51" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J51" t="str">
         <f t="shared" si="14"/>
         <v>{{ notice.ReportReceivedDate ? notice.ReportReceivedDate : "n/a" }}</v>
       </c>
-      <c r="K48" t="str">
+      <c r="K51" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Report Received Date&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.ReportReceivedDate ? notice.ReportReceivedDate : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E52" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F52" t="s">
+        <v>93</v>
+      </c>
+      <c r="G52" t="s">
+        <v>93</v>
+      </c>
+      <c r="H52" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L48" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Report Received Date&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.ReportReceivedDate ? notice.ReportReceivedDate : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E49" t="str">
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I52" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" t="s">
-        <v>93</v>
-      </c>
-      <c r="H49" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I49" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J49" t="str">
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J52" t="str">
         <f t="shared" si="14"/>
         <v>{{ notice.Component ? notice.Component : "n/a" }}</v>
       </c>
-      <c r="K49" t="str">
+      <c r="K52" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Component&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Component ? notice.Component : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E53" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F53" t="s">
+        <v>94</v>
+      </c>
+      <c r="G53" t="s">
+        <v>94</v>
+      </c>
+      <c r="H53" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L49" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Component&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Component ? notice.Component : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E50" t="str">
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I53" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F50" t="s">
-        <v>94</v>
-      </c>
-      <c r="G50" t="s">
-        <v>94</v>
-      </c>
-      <c r="H50" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I50" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J50" t="str">
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J53" t="str">
         <f t="shared" si="14"/>
         <v>{{ notice.Summary ? notice.Summary : "n/a" }}</v>
       </c>
-      <c r="K50" t="str">
+      <c r="K53" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Summary&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Summary ? notice.Summary : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E54" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F54" t="s">
+        <v>95</v>
+      </c>
+      <c r="G54" t="s">
+        <v>101</v>
+      </c>
+      <c r="H54" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L50" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Summary&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Summary ? notice.Summary : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E51" t="str">
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I54" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F51" t="s">
-        <v>95</v>
-      </c>
-      <c r="G51" t="s">
-        <v>101</v>
-      </c>
-      <c r="H51" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I51" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J51" t="str">
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J54" t="str">
         <f t="shared" si="14"/>
         <v>{{ notice.Conequence ? notice.Conequence : "n/a" }}</v>
       </c>
-      <c r="K51" t="str">
+      <c r="K54" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Consequence&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Conequence ? notice.Conequence : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E55" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F55" t="s">
+        <v>96</v>
+      </c>
+      <c r="G55" t="s">
+        <v>96</v>
+      </c>
+      <c r="H55" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L51" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Consequence&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Conequence ? notice.Conequence : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E52" t="str">
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I55" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F52" t="s">
-        <v>96</v>
-      </c>
-      <c r="G52" t="s">
-        <v>96</v>
-      </c>
-      <c r="H52" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I52" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J52" t="str">
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J55" t="str">
         <f t="shared" si="14"/>
         <v>{{ notice.Remedy ? notice.Remedy : "n/a" }}</v>
       </c>
-      <c r="K52" t="str">
+      <c r="K55" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="15"/>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Remedy&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Remedy ? notice.Remedy : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E56" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;p class="recall-heading" &gt;</v>
+      </c>
+      <c r="F56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" t="s">
+        <v>97</v>
+      </c>
+      <c r="H56" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L52" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Remedy&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Remedy ? notice.Remedy : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E53" t="str">
+        <v>&lt;/p&gt;</v>
+      </c>
+      <c r="I56" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G53" t="s">
-        <v>97</v>
-      </c>
-      <c r="H53" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I53" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J53" t="str">
+        <v>&lt;p class="recall-data" &gt;</v>
+      </c>
+      <c r="J56" t="str">
         <f t="shared" si="14"/>
         <v>{{ notice.Notes ? notice.Notes : "n/a" }}</v>
       </c>
-      <c r="K53" t="str">
-        <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L53" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Notes&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Notes ? notice.Notes : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E54" t="str">
-        <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F54" t="s">
-        <v>98</v>
-      </c>
-      <c r="G54" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I54" t="str">
+      <c r="K56" t="str">
         <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J54" t="str">
-        <f t="shared" si="14"/>
-        <v>{{ notice.ModelYear ? notice.ModelYear : "n/a" }}</v>
-      </c>
-      <c r="K54" t="str">
-        <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L54" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Model Year&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.ModelYear ? notice.ModelYear : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E55" t="str">
-        <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F55" t="s">
-        <v>52</v>
-      </c>
-      <c r="G55" t="s">
-        <v>52</v>
-      </c>
-      <c r="H55" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I55" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J55" t="str">
-        <f t="shared" si="14"/>
-        <v>{{ notice.Make ? notice.Make : "n/a" }}</v>
-      </c>
-      <c r="K55" t="str">
-        <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="L55" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Make&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Make ? notice.Make : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E56" t="str">
-        <f t="shared" si="12"/>
-        <v>&lt;span class="recall-heading" &gt;</v>
-      </c>
-      <c r="F56" t="s">
-        <v>53</v>
-      </c>
-      <c r="G56" t="s">
-        <v>53</v>
-      </c>
-      <c r="H56" t="str">
-        <f t="shared" si="10"/>
-        <v>&lt;/span&gt;</v>
-      </c>
-      <c r="I56" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;span class="recall-data" &gt;</v>
-      </c>
-      <c r="J56" t="str">
-        <f t="shared" si="14"/>
-        <v>{{ notice.Model ? notice.Model : "n/a" }}</v>
-      </c>
-      <c r="K56" t="str">
-        <f t="shared" si="11"/>
-        <v>&lt;/span&gt;</v>
+        <v>&lt;/p&gt;</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="15"/>
-        <v>&lt;div class="recall-grp" &gt;&lt;span class="recall-heading" &gt;Model&lt;/span&gt;&lt;span class="recall-data" &gt;{{ notice.Model ? notice.Model : "n/a" }}&lt;/span&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="recall-grp" &gt;&lt;p class="recall-heading" &gt;Notes&lt;/p&gt;&lt;p class="recall-data" &gt;{{ notice.Notes ? notice.Notes : "n/a" }}&lt;/p&gt;&lt;/div&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>